<commit_message>
Import Scripts based on OpenPyXL
</commit_message>
<xml_diff>
--- a/.init/fiscal.xlsx
+++ b/.init/fiscal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Coding\django-yolobuilds\.init\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21708E2F-072C-4611-9890-3E5457E6B26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F944AE04-B3D4-4498-AF88-CE75FA8B2D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13896" yWindow="0" windowWidth="9252" windowHeight="12504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="accounts" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="476">
   <si>
     <t>General Fund</t>
   </si>
@@ -1237,9 +1237,6 @@
     <t>County Service Area</t>
   </si>
   <si>
-    <t>2975-BD5009</t>
-  </si>
-  <si>
     <t>60312975120019401310</t>
   </si>
   <si>
@@ -1487,6 +1484,9 @@
   </si>
   <si>
     <t>Only use at the direction of management.</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -2046,7 +2046,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2124,19 +2124,16 @@
     <xf numFmtId="10" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2186,18 +2183,14 @@
   </cellStyles>
   <dxfs count="36">
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -2247,6 +2240,20 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2515,16 +2522,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FF000000"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
@@ -2568,57 +2565,57 @@
     <sortCondition ref="A1:A38"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="6" xr3:uid="{A36371C9-1ED7-4956-A933-3FB3510B2E6E}" name="id" dataDxfId="33"/>
-    <tableColumn id="8" xr3:uid="{775FB684-8436-4935-AFC0-BF15AC6A2D0B}" name="fund" dataDxfId="32"/>
-    <tableColumn id="9" xr3:uid="{74A33601-C14D-47D2-958E-CC084A6C2E7A}" name="fund_label" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{A109FF24-3A47-4179-9EA1-0A363C921F6E}" name="share" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{1AE7FC7D-C7E8-4911-ABD5-0D4D24A624BD}" name="unit" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{D2DF4AEA-1359-4A36-9F8F-DBD2A11615E2}" name="unit_label" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{FD5E3650-2F9F-4CDF-816F-145B8D2BD6FE}" name="unit_description" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{3E3D4E34-3247-4D64-B6BB-96BE1D0B0998}" name="cost_center" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{966172B4-DFF5-4D39-9854-B206F0B9B101}" name="gl_account" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{7F5A11D0-41E3-460B-861D-4A4DD72A7B91}" name="cams" dataDxfId="24"/>
-    <tableColumn id="13" xr3:uid="{098F32BB-089B-4345-8803-2A67F282B8AB}" name="Infor Activity" dataDxfId="23"/>
-    <tableColumn id="14" xr3:uid="{2EF6164A-AACC-4E96-AEFF-2A04ADE82E0B}" name="Infor Account Category" dataDxfId="22"/>
-    <tableColumn id="12" xr3:uid="{F1C5C1C3-295F-4B6A-A0D8-6AD64682BF30}" name="ledger" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{A36371C9-1ED7-4956-A933-3FB3510B2E6E}" name="id" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{775FB684-8436-4935-AFC0-BF15AC6A2D0B}" name="fund" dataDxfId="33"/>
+    <tableColumn id="9" xr3:uid="{74A33601-C14D-47D2-958E-CC084A6C2E7A}" name="fund_label" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{A109FF24-3A47-4179-9EA1-0A363C921F6E}" name="share" dataDxfId="31"/>
+    <tableColumn id="10" xr3:uid="{1AE7FC7D-C7E8-4911-ABD5-0D4D24A624BD}" name="unit" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{D2DF4AEA-1359-4A36-9F8F-DBD2A11615E2}" name="unit_label" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{FD5E3650-2F9F-4CDF-816F-145B8D2BD6FE}" name="unit_description" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{3E3D4E34-3247-4D64-B6BB-96BE1D0B0998}" name="cost_center" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{966172B4-DFF5-4D39-9854-B206F0B9B101}" name="gl_account" dataDxfId="26"/>
+    <tableColumn id="11" xr3:uid="{7F5A11D0-41E3-460B-861D-4A4DD72A7B91}" name="cams" dataDxfId="25"/>
+    <tableColumn id="13" xr3:uid="{098F32BB-089B-4345-8803-2A67F282B8AB}" name="Infor Activity" dataDxfId="24"/>
+    <tableColumn id="14" xr3:uid="{2EF6164A-AACC-4E96-AEFF-2A04ADE82E0B}" name="Infor Account Category" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{F1C5C1C3-295F-4B6A-A0D8-6AD64682BF30}" name="ledger" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D85CC903-F636-4C4A-A831-C42F96AA99CB}" name="Table3" displayName="Table3" ref="A1:N139" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D85CC903-F636-4C4A-A831-C42F96AA99CB}" name="Table3" displayName="Table3" ref="A1:N139" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:N139" xr:uid="{B3956DC0-773A-470A-AB5E-798CB1F07FBC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N139">
     <sortCondition ref="A1:A139"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="16" xr3:uid="{53AA541E-CFBC-4EC3-A314-B49A000EE89B}" name="id" dataDxfId="18"/>
-    <tableColumn id="17" xr3:uid="{82695AFC-E86E-46DA-B6B6-CD756A1CEA4E}" name="fee_account" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{6ED7D1AC-A7DD-4964-920C-8D78B8066079}" name="fee_group" dataDxfId="16"/>
-    <tableColumn id="1" xr3:uid="{FF38A444-BC61-478D-B7E8-D54F42F7BD6B}" name="fee_type" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{840C0681-906D-41CF-8941-B1EE10C3859E}" name="policy" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{20438A78-0406-4000-8560-52D2BC2D45AA}" name="authorization" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{7A6A4488-BC83-4988-B03A-1E757A26F3D6}" name="adopted" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{4F9606B4-E13E-4D9F-92C9-BE41B6669C75}" name="revised" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{39FA530A-7500-41FF-9C7E-6DB8AADAD184}" name="expires" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{09AA4BF6-9396-4563-9058-49272424166F}" name="tier_base_qty" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{958710A4-FC54-434A-B371-385C30E60BF1}" name="tier_base_fee" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{EAEAA671-06AE-47B6-8818-161514EE7529}" name="rate" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{149011A9-C6F4-4E88-9F35-D40C7D3127DF}" name="units" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{4C032D57-28D2-4B05-9556-AA5592ED152B}" name="rate_check" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{53AA541E-CFBC-4EC3-A314-B49A000EE89B}" name="Column1" dataDxfId="19"/>
+    <tableColumn id="17" xr3:uid="{82695AFC-E86E-46DA-B6B6-CD756A1CEA4E}" name="fee_account" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{6ED7D1AC-A7DD-4964-920C-8D78B8066079}" name="fee_group" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{FF38A444-BC61-478D-B7E8-D54F42F7BD6B}" name="fee_type" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{840C0681-906D-41CF-8941-B1EE10C3859E}" name="policy" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{20438A78-0406-4000-8560-52D2BC2D45AA}" name="authorization" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{7A6A4488-BC83-4988-B03A-1E757A26F3D6}" name="adopted" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{4F9606B4-E13E-4D9F-92C9-BE41B6669C75}" name="revised" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{39FA530A-7500-41FF-9C7E-6DB8AADAD184}" name="expires" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{09AA4BF6-9396-4563-9058-49272424166F}" name="tier_base_qty" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{958710A4-FC54-434A-B371-385C30E60BF1}" name="tier_base_fee" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{EAEAA671-06AE-47B6-8818-161514EE7529}" name="rate" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{149011A9-C6F4-4E88-9F35-D40C7D3127DF}" name="units" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{4C032D57-28D2-4B05-9556-AA5592ED152B}" name="rate_check" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{32DEFFCE-B2B2-46D8-857E-69F936A677E6}" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{32DEFFCE-B2B2-46D8-857E-69F936A677E6}" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:C8" xr:uid="{32DEFFCE-B2B2-46D8-857E-69F936A677E6}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C83F5F05-6046-46E9-A1E1-3541B5D40B45}" name="id" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{6C0B881C-90B5-433A-82EB-1B4A65DA8DD1}" name="method" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{E20501A0-DD84-4EF5-B4CE-42C0CD6AD573}" name="policy" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{C83F5F05-6046-46E9-A1E1-3541B5D40B45}" name="id" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{6C0B881C-90B5-433A-82EB-1B4A65DA8DD1}" name="method" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{E20501A0-DD84-4EF5-B4CE-42C0CD6AD573}" name="policy" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2931,8 +2928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78991DAA-9181-470A-9377-ABCE3748D609}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2986,10 +2983,10 @@
         <v>376</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>446</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>447</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>375</v>
@@ -2998,9 +2995,7 @@
       <c r="O1" s="3"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="12">
-        <v>101</v>
-      </c>
+      <c r="A2" s="12"/>
       <c r="B2" s="4" t="s">
         <v>374</v>
       </c>
@@ -3011,16 +3006,16 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>422</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>421</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>421</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>423</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>367</v>
@@ -3029,15 +3024,13 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
-        <v>102</v>
-      </c>
+      <c r="A3" s="12"/>
       <c r="B3" s="4" t="s">
         <v>374</v>
       </c>
@@ -3048,35 +3041,33 @@
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>448</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="4"/>
+      <c r="H3" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="4" t="s">
-        <v>450</v>
-      </c>
       <c r="I3" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="J3" s="10"/>
+        <v>419</v>
+      </c>
+      <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>453</v>
-      </c>
       <c r="M3" s="10" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
-        <v>103</v>
-      </c>
+      <c r="A4" s="12"/>
       <c r="B4" s="4" t="s">
         <v>374</v>
       </c>
@@ -3098,18 +3089,16 @@
       <c r="H4" s="4">
         <v>120002</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
-        <v>104</v>
-      </c>
+      <c r="A5" s="12"/>
       <c r="B5" s="4">
         <v>1001</v>
       </c>
@@ -3123,7 +3112,7 @@
         <v>2971</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>9</v>
@@ -3135,7 +3124,7 @@
         <v>352</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
@@ -3146,9 +3135,7 @@
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
-        <v>105</v>
-      </c>
+      <c r="A6" s="12"/>
       <c r="B6" s="4">
         <v>1001</v>
       </c>
@@ -3185,9 +3172,7 @@
       <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
-        <v>106</v>
-      </c>
+      <c r="A7" s="12"/>
       <c r="B7" s="4" t="s">
         <v>374</v>
       </c>
@@ -3201,7 +3186,7 @@
         <v>365</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>9</v>
@@ -3213,20 +3198,18 @@
         <v>384</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="12">
-        <v>107</v>
-      </c>
+      <c r="A8" s="12"/>
       <c r="B8" s="4" t="s">
         <v>374</v>
       </c>
@@ -3240,7 +3223,7 @@
         <v>365</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>9</v>
@@ -3249,21 +3232,19 @@
         <v>120003</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="12">
-        <v>108</v>
-      </c>
+      <c r="A9" s="12"/>
       <c r="B9" s="4">
         <v>1001</v>
       </c>
@@ -3287,16 +3268,14 @@
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="12">
-        <v>109</v>
-      </c>
+      <c r="A10" s="12"/>
       <c r="B10" s="4">
         <v>1001</v>
       </c>
@@ -3320,16 +3299,14 @@
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="12">
-        <v>110</v>
-      </c>
+      <c r="A11" s="12"/>
       <c r="B11" s="4">
         <v>1001</v>
       </c>
@@ -3366,11 +3343,9 @@
       <c r="O11" s="3"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="12">
-        <v>111</v>
-      </c>
+      <c r="A12" s="12"/>
       <c r="B12" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>302</v>
@@ -3379,7 +3354,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>304</v>
@@ -3388,26 +3363,24 @@
         <v>306</v>
       </c>
       <c r="H12" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="J12" s="4" t="s">
         <v>403</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>404</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="12">
-        <v>112</v>
-      </c>
+      <c r="A13" s="12"/>
       <c r="B13" s="4" t="s">
         <v>364</v>
       </c>
@@ -3423,16 +3396,16 @@
       <c r="F13" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="G13" s="10"/>
+      <c r="G13" s="4"/>
       <c r="H13" s="4" t="s">
         <v>366</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
       <c r="M13" s="10" t="s">
         <v>368</v>
       </c>
@@ -3440,9 +3413,7 @@
       <c r="O13" s="3"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="12">
-        <v>113</v>
-      </c>
+      <c r="A14" s="12"/>
       <c r="B14" s="4">
         <v>1001</v>
       </c>
@@ -3464,18 +3435,16 @@
       <c r="H14" s="4">
         <v>120015</v>
       </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="12">
-        <v>201</v>
-      </c>
+      <c r="A15" s="12"/>
       <c r="B15" s="4">
         <v>2030</v>
       </c>
@@ -3497,18 +3466,16 @@
       <c r="H15" s="4">
         <v>120026</v>
       </c>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="12">
-        <v>202</v>
-      </c>
+      <c r="A16" s="12"/>
       <c r="B16" s="4">
         <v>2030</v>
       </c>
@@ -3530,18 +3497,16 @@
       <c r="H16" s="4">
         <v>120027</v>
       </c>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="12">
-        <v>203</v>
-      </c>
+      <c r="A17" s="12"/>
       <c r="B17" s="4">
         <v>2030</v>
       </c>
@@ -3555,7 +3520,7 @@
         <v>3011</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>22</v>
@@ -3564,27 +3529,25 @@
         <v>120028</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J17" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="M17" s="4" t="s">
         <v>454</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>455</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="12">
-        <v>204</v>
-      </c>
+      <c r="A18" s="12"/>
       <c r="B18" s="4">
         <v>2030</v>
       </c>
@@ -3598,7 +3561,7 @@
         <v>3011</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>22</v>
@@ -3607,21 +3570,19 @@
         <v>120028</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="12">
-        <v>205</v>
-      </c>
+      <c r="A19" s="12"/>
       <c r="B19" s="4">
         <v>2030</v>
       </c>
@@ -3635,7 +3596,7 @@
         <v>3011</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>22</v>
@@ -3644,23 +3605,21 @@
         <v>120028</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="12">
-        <v>206</v>
-      </c>
+      <c r="A20" s="12"/>
       <c r="B20" s="4">
         <v>2030</v>
       </c>
@@ -3674,7 +3633,7 @@
         <v>3011</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>22</v>
@@ -3683,21 +3642,19 @@
         <v>120028</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="12">
-        <v>207</v>
-      </c>
+      <c r="A21" s="12"/>
       <c r="B21" s="4">
         <v>2030</v>
       </c>
@@ -3707,9 +3664,11 @@
       <c r="D21" s="8">
         <v>1</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4">
+        <v>3011</v>
+      </c>
       <c r="F21" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>22</v>
@@ -3718,27 +3677,25 @@
         <v>120028</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J21" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="K21" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="L21" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="L21" s="4" t="s">
-        <v>453</v>
-      </c>
       <c r="M21" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="12">
-        <v>208</v>
-      </c>
+      <c r="A22" s="12"/>
       <c r="B22" s="4">
         <v>2030</v>
       </c>
@@ -3752,7 +3709,7 @@
         <v>3011</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>22</v>
@@ -3761,23 +3718,21 @@
         <v>120028</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="12">
-        <v>209</v>
-      </c>
+      <c r="A23" s="12"/>
       <c r="B23" s="4">
         <v>2030</v>
       </c>
@@ -3799,23 +3754,21 @@
       <c r="H23" s="4">
         <v>120029</v>
       </c>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="12">
-        <v>210</v>
-      </c>
+      <c r="A24" s="12"/>
       <c r="B24" s="4" t="s">
         <v>387</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D24" s="8">
         <v>1</v>
@@ -3827,7 +3780,7 @@
         <v>391</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>389</v>
@@ -3843,9 +3796,7 @@
       <c r="O24" s="3"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="24">
-        <v>601</v>
-      </c>
+      <c r="A25" s="24"/>
       <c r="B25" s="25">
         <v>6031</v>
       </c>
@@ -3867,24 +3818,18 @@
       <c r="H25" s="25" t="s">
         <v>381</v>
       </c>
-      <c r="I25" s="25" t="s">
-        <v>354</v>
-      </c>
-      <c r="J25" s="25" t="s">
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="25" t="s">
         <v>392</v>
-      </c>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25" t="s">
-        <v>393</v>
       </c>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="24">
-        <v>602</v>
-      </c>
+      <c r="A26" s="24"/>
       <c r="B26" s="25">
         <v>6031</v>
       </c>
@@ -3912,8 +3857,8 @@
       <c r="J26" s="25" t="s">
         <v>385</v>
       </c>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
       <c r="M26" s="25" t="s">
         <v>386</v>
       </c>
@@ -3921,9 +3866,7 @@
       <c r="O26" s="3"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="24">
-        <v>603</v>
-      </c>
+      <c r="A27" s="24"/>
       <c r="B27" s="4">
         <v>6031</v>
       </c>
@@ -3960,9 +3903,7 @@
       <c r="O27" s="3"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="24">
-        <v>604</v>
-      </c>
+      <c r="A28" s="24"/>
       <c r="B28" s="25" t="s">
         <v>370</v>
       </c>
@@ -3976,22 +3917,22 @@
         <v>383</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G28" s="25" t="s">
         <v>357</v>
       </c>
       <c r="H28" s="25" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I28" s="25" t="s">
         <v>354</v>
       </c>
       <c r="J28" s="25" t="s">
-        <v>399</v>
-      </c>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
+        <v>398</v>
+      </c>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
       <c r="M28" s="25" t="s">
         <v>355</v>
       </c>
@@ -3999,11 +3940,9 @@
       <c r="O28" s="3"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="24">
-        <v>701</v>
-      </c>
+      <c r="A29" s="24"/>
       <c r="B29" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>303</v>
@@ -4012,7 +3951,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>305</v>
@@ -4021,7 +3960,7 @@
         <v>307</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>354</v>
@@ -4030,15 +3969,13 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="24">
-        <v>801</v>
-      </c>
+      <c r="A30" s="24"/>
       <c r="B30" s="4" t="s">
         <v>370</v>
       </c>
@@ -4052,13 +3989,13 @@
         <v>383</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>384</v>
@@ -4067,15 +4004,13 @@
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="24">
-        <v>802</v>
-      </c>
+      <c r="A31" s="24"/>
       <c r="B31" s="4" t="s">
         <v>370</v>
       </c>
@@ -4089,13 +4024,13 @@
         <v>383</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>354</v>
@@ -4104,15 +4039,13 @@
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" s="24">
-        <v>803</v>
-      </c>
+      <c r="A32" s="24"/>
       <c r="B32" s="4" t="s">
         <v>370</v>
       </c>
@@ -4123,33 +4056,31 @@
         <v>1</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A33" s="24">
-        <v>804</v>
-      </c>
+      <c r="A33" s="24"/>
       <c r="B33" s="4">
         <v>6031</v>
       </c>
@@ -4163,7 +4094,7 @@
         <v>2975</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>17</v>
@@ -4178,15 +4109,13 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A34" s="24">
-        <v>805</v>
-      </c>
+      <c r="A34" s="24"/>
       <c r="B34" s="4" t="s">
         <v>370</v>
       </c>
@@ -4197,33 +4126,31 @@
         <v>1</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A35" s="24">
-        <v>806</v>
-      </c>
+      <c r="A35" s="24"/>
       <c r="B35" s="4" t="s">
         <v>370</v>
       </c>
@@ -4234,33 +4161,31 @@
         <v>1</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A36" s="24">
-        <v>901</v>
-      </c>
+      <c r="A36" s="24"/>
       <c r="B36" s="4" t="s">
         <v>370</v>
       </c>
@@ -4272,7 +4197,7 @@
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="4" t="s">
@@ -4289,9 +4214,7 @@
       <c r="O36" s="3"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A37" s="24">
-        <v>902</v>
-      </c>
+      <c r="A37" s="24"/>
       <c r="B37" s="4" t="s">
         <v>370</v>
       </c>
@@ -4303,7 +4226,7 @@
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="4" t="s">
@@ -4320,9 +4243,7 @@
       <c r="O37" s="3"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A38" s="24">
-        <v>903</v>
-      </c>
+      <c r="A38" s="24"/>
       <c r="B38" s="4" t="s">
         <v>370</v>
       </c>
@@ -4334,7 +4255,7 @@
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="4" t="s">
@@ -4365,8 +4286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682FC1F9-8F65-4C37-A089-78E25FAF4B7B}">
   <dimension ref="A1:O139"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4393,16 +4314,16 @@
   <sheetData>
     <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>25</v>
+        <v>475</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>339</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>287</v>
@@ -4429,16 +4350,14 @@
         <v>280</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="18">
-        <v>1301</v>
-      </c>
+      <c r="A2" s="18"/>
       <c r="B2" s="18">
         <v>13</v>
       </c>
@@ -4475,9 +4394,7 @@
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="18">
-        <v>1302</v>
-      </c>
+      <c r="A3" s="18"/>
       <c r="B3" s="18">
         <v>13</v>
       </c>
@@ -4514,9 +4431,7 @@
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="18">
-        <v>1303</v>
-      </c>
+      <c r="A4" s="18"/>
       <c r="B4" s="18">
         <v>13</v>
       </c>
@@ -4555,9 +4470,7 @@
       <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="18">
-        <v>1304</v>
-      </c>
+      <c r="A5" s="18"/>
       <c r="B5" s="18">
         <v>13</v>
       </c>
@@ -4594,9 +4507,7 @@
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="18">
-        <v>1305</v>
-      </c>
+      <c r="A6" s="18"/>
       <c r="B6" s="18">
         <v>13</v>
       </c>
@@ -4633,9 +4544,7 @@
       <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="18">
-        <v>1306</v>
-      </c>
+      <c r="A7" s="18"/>
       <c r="B7" s="18">
         <v>13</v>
       </c>
@@ -4672,9 +4581,7 @@
       <c r="O7" s="3"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="18">
-        <v>1307</v>
-      </c>
+      <c r="A8" s="18"/>
       <c r="B8" s="18">
         <v>13</v>
       </c>
@@ -4711,9 +4618,7 @@
       <c r="O8" s="3"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="18">
-        <v>1308</v>
-      </c>
+      <c r="A9" s="18"/>
       <c r="B9" s="18">
         <v>13</v>
       </c>
@@ -4750,9 +4655,7 @@
       <c r="O9" s="3"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="18">
-        <v>1309</v>
-      </c>
+      <c r="A10" s="18"/>
       <c r="B10" s="18">
         <v>13</v>
       </c>
@@ -4791,9 +4694,7 @@
       <c r="O10" s="3"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="18">
-        <v>1310</v>
-      </c>
+      <c r="A11" s="18"/>
       <c r="B11" s="18">
         <v>13</v>
       </c>
@@ -4832,9 +4733,7 @@
       <c r="O11" s="3"/>
     </row>
     <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="18">
-        <v>1801</v>
-      </c>
+      <c r="A12" s="18"/>
       <c r="B12" s="20" t="s">
         <v>338</v>
       </c>
@@ -4873,9 +4772,7 @@
       <c r="O12" s="3"/>
     </row>
     <row r="13" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="18">
-        <v>1901</v>
-      </c>
+      <c r="A13" s="18"/>
       <c r="B13" s="20">
         <v>19</v>
       </c>
@@ -4914,9 +4811,7 @@
       <c r="O13" s="3"/>
     </row>
     <row r="14" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="18">
-        <v>2101</v>
-      </c>
+      <c r="A14" s="18"/>
       <c r="B14" s="9">
         <v>21</v>
       </c>
@@ -4953,9 +4848,7 @@
       <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="18">
-        <v>2102</v>
-      </c>
+      <c r="A15" s="18"/>
       <c r="B15" s="9">
         <v>21</v>
       </c>
@@ -4994,9 +4887,7 @@
       <c r="O15" s="3"/>
     </row>
     <row r="16" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="18">
-        <v>2103</v>
-      </c>
+      <c r="A16" s="18"/>
       <c r="B16" s="9">
         <v>21</v>
       </c>
@@ -5035,9 +4926,7 @@
       <c r="O16" s="3"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="18">
-        <v>2104</v>
-      </c>
+      <c r="A17" s="18"/>
       <c r="B17" s="9">
         <v>21</v>
       </c>
@@ -5076,9 +4965,7 @@
       <c r="O17" s="3"/>
     </row>
     <row r="18" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="18">
-        <v>2105</v>
-      </c>
+      <c r="A18" s="18"/>
       <c r="B18" s="9">
         <v>21</v>
       </c>
@@ -5115,9 +5002,7 @@
       <c r="O18" s="3"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="18">
-        <v>2106</v>
-      </c>
+      <c r="A19" s="18"/>
       <c r="B19" s="9">
         <v>21</v>
       </c>
@@ -5156,9 +5041,7 @@
       <c r="O19" s="3"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="18">
-        <v>2107</v>
-      </c>
+      <c r="A20" s="18"/>
       <c r="B20" s="9">
         <v>21</v>
       </c>
@@ -5195,9 +5078,7 @@
       <c r="O20" s="3"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="18">
-        <v>2108</v>
-      </c>
+      <c r="A21" s="18"/>
       <c r="B21" s="9">
         <v>21</v>
       </c>
@@ -5234,9 +5115,7 @@
       <c r="O21" s="3"/>
     </row>
     <row r="22" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="18">
-        <v>2109</v>
-      </c>
+      <c r="A22" s="18"/>
       <c r="B22" s="9">
         <v>21</v>
       </c>
@@ -5275,9 +5154,7 @@
       <c r="O22" s="3"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="18">
-        <v>2110</v>
-      </c>
+      <c r="A23" s="18"/>
       <c r="B23" s="9">
         <v>21</v>
       </c>
@@ -5314,9 +5191,7 @@
       <c r="O23" s="3"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="18">
-        <v>2111</v>
-      </c>
+      <c r="A24" s="18"/>
       <c r="B24" s="9">
         <v>21</v>
       </c>
@@ -5355,9 +5230,7 @@
       <c r="O24" s="3"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="18">
-        <v>2112</v>
-      </c>
+      <c r="A25" s="18"/>
       <c r="B25" s="9">
         <v>21</v>
       </c>
@@ -5396,9 +5269,7 @@
       <c r="O25" s="3"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="18">
-        <v>2113</v>
-      </c>
+      <c r="A26" s="18"/>
       <c r="B26" s="9">
         <v>21</v>
       </c>
@@ -5435,9 +5306,7 @@
       <c r="O26" s="3"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="18">
-        <v>2114</v>
-      </c>
+      <c r="A27" s="18"/>
       <c r="B27" s="9">
         <v>21</v>
       </c>
@@ -5476,9 +5345,7 @@
       <c r="O27" s="3"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="18">
-        <v>2115</v>
-      </c>
+      <c r="A28" s="18"/>
       <c r="B28" s="9">
         <v>21</v>
       </c>
@@ -5515,9 +5382,7 @@
       <c r="O28" s="3"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="18">
-        <v>2201</v>
-      </c>
+      <c r="A29" s="18"/>
       <c r="B29" s="22">
         <v>22</v>
       </c>
@@ -5556,9 +5421,7 @@
       <c r="O29" s="3"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="18">
-        <v>2202</v>
-      </c>
+      <c r="A30" s="18"/>
       <c r="B30" s="22">
         <v>22</v>
       </c>
@@ -5595,9 +5458,7 @@
       <c r="O30" s="3"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="18">
-        <v>2203</v>
-      </c>
+      <c r="A31" s="18"/>
       <c r="B31" s="22">
         <v>22</v>
       </c>
@@ -5634,9 +5495,7 @@
       <c r="O31" s="3"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" s="18">
-        <v>2204</v>
-      </c>
+      <c r="A32" s="18"/>
       <c r="B32" s="22">
         <v>22</v>
       </c>
@@ -5673,9 +5532,7 @@
       <c r="O32" s="3"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A33" s="18">
-        <v>2205</v>
-      </c>
+      <c r="A33" s="18"/>
       <c r="B33" s="22">
         <v>22</v>
       </c>
@@ -5712,9 +5569,7 @@
       <c r="O33" s="3"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A34" s="18">
-        <v>2206</v>
-      </c>
+      <c r="A34" s="18"/>
       <c r="B34" s="22">
         <v>22</v>
       </c>
@@ -5753,9 +5608,7 @@
       <c r="O34" s="3"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A35" s="18">
-        <v>2207</v>
-      </c>
+      <c r="A35" s="18"/>
       <c r="B35" s="22">
         <v>22</v>
       </c>
@@ -5792,9 +5645,7 @@
       <c r="O35" s="3"/>
     </row>
     <row r="36" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="18">
-        <v>2208</v>
-      </c>
+      <c r="A36" s="18"/>
       <c r="B36" s="22">
         <v>22</v>
       </c>
@@ -5833,9 +5684,7 @@
       <c r="O36" s="3"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A37" s="18">
-        <v>2209</v>
-      </c>
+      <c r="A37" s="18"/>
       <c r="B37" s="22">
         <v>22</v>
       </c>
@@ -5872,9 +5721,7 @@
       <c r="O37" s="3"/>
     </row>
     <row r="38" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="18">
-        <v>2301</v>
-      </c>
+      <c r="A38" s="18"/>
       <c r="B38" s="21">
         <v>23</v>
       </c>
@@ -5913,9 +5760,7 @@
       <c r="O38" s="3"/>
     </row>
     <row r="39" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="18">
-        <v>2302</v>
-      </c>
+      <c r="A39" s="18"/>
       <c r="B39" s="21">
         <v>23</v>
       </c>
@@ -5954,9 +5799,7 @@
       <c r="O39" s="3"/>
     </row>
     <row r="40" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="18">
-        <v>2303</v>
-      </c>
+      <c r="A40" s="18"/>
       <c r="B40" s="21">
         <v>23</v>
       </c>
@@ -5995,9 +5838,7 @@
       <c r="O40" s="3"/>
     </row>
     <row r="41" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="18">
-        <v>2304</v>
-      </c>
+      <c r="A41" s="18"/>
       <c r="B41" s="21">
         <v>23</v>
       </c>
@@ -6036,9 +5877,7 @@
       <c r="O41" s="3"/>
     </row>
     <row r="42" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="18">
-        <v>2305</v>
-      </c>
+      <c r="A42" s="18"/>
       <c r="B42" s="21">
         <v>23</v>
       </c>
@@ -6077,9 +5916,7 @@
       <c r="O42" s="3"/>
     </row>
     <row r="43" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="18">
-        <v>2306</v>
-      </c>
+      <c r="A43" s="18"/>
       <c r="B43" s="21">
         <v>23</v>
       </c>
@@ -6118,9 +5955,7 @@
       <c r="O43" s="3"/>
     </row>
     <row r="44" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A44" s="18">
-        <v>2307</v>
-      </c>
+      <c r="A44" s="18"/>
       <c r="B44" s="21">
         <v>23</v>
       </c>
@@ -6159,9 +5994,7 @@
       <c r="O44" s="3"/>
     </row>
     <row r="45" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="18">
-        <v>2311</v>
-      </c>
+      <c r="A45" s="18"/>
       <c r="B45" s="21">
         <v>23</v>
       </c>
@@ -6198,9 +6031,7 @@
       <c r="O45" s="3"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A46" s="18">
-        <v>2312</v>
-      </c>
+      <c r="A46" s="18"/>
       <c r="B46" s="21">
         <v>23</v>
       </c>
@@ -6237,9 +6068,7 @@
       <c r="O46" s="3"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A47" s="18">
-        <v>2313</v>
-      </c>
+      <c r="A47" s="18"/>
       <c r="B47" s="21">
         <v>23</v>
       </c>
@@ -6276,9 +6105,7 @@
       <c r="O47" s="3"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A48" s="18">
-        <v>2314</v>
-      </c>
+      <c r="A48" s="18"/>
       <c r="B48" s="21">
         <v>23</v>
       </c>
@@ -6315,9 +6142,7 @@
       <c r="O48" s="3"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A49" s="18">
-        <v>2315</v>
-      </c>
+      <c r="A49" s="18"/>
       <c r="B49" s="21">
         <v>23</v>
       </c>
@@ -6354,9 +6179,7 @@
       <c r="O49" s="3"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A50" s="18">
-        <v>2316</v>
-      </c>
+      <c r="A50" s="18"/>
       <c r="B50" s="21">
         <v>23</v>
       </c>
@@ -6393,9 +6216,7 @@
       <c r="O50" s="3"/>
     </row>
     <row r="51" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="18">
-        <v>2317</v>
-      </c>
+      <c r="A51" s="18"/>
       <c r="B51" s="21">
         <v>23</v>
       </c>
@@ -6432,9 +6253,7 @@
       <c r="O51" s="3"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A52" s="18">
-        <v>2318</v>
-      </c>
+      <c r="A52" s="18"/>
       <c r="B52" s="21">
         <v>23</v>
       </c>
@@ -6471,9 +6290,7 @@
       <c r="O52" s="3"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A53" s="18">
-        <v>2319</v>
-      </c>
+      <c r="A53" s="18"/>
       <c r="B53" s="21">
         <v>23</v>
       </c>
@@ -6510,9 +6327,7 @@
       <c r="O53" s="3"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A54" s="18">
-        <v>2320</v>
-      </c>
+      <c r="A54" s="18"/>
       <c r="B54" s="21">
         <v>23</v>
       </c>
@@ -6549,9 +6364,7 @@
       <c r="O54" s="3"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A55" s="18">
-        <v>2001</v>
-      </c>
+      <c r="A55" s="18"/>
       <c r="B55" s="21">
         <v>23</v>
       </c>
@@ -6588,9 +6401,7 @@
       <c r="O55" s="3"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A56" s="18">
-        <v>2321</v>
-      </c>
+      <c r="A56" s="18"/>
       <c r="B56" s="21">
         <v>23</v>
       </c>
@@ -6627,9 +6438,7 @@
       <c r="O56" s="3"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A57" s="18">
-        <v>2322</v>
-      </c>
+      <c r="A57" s="18"/>
       <c r="B57" s="21">
         <v>23</v>
       </c>
@@ -6666,9 +6475,7 @@
       <c r="O57" s="3"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A58" s="18">
-        <v>2323</v>
-      </c>
+      <c r="A58" s="18"/>
       <c r="B58" s="21">
         <v>23</v>
       </c>
@@ -6705,9 +6512,7 @@
       <c r="O58" s="3"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A59" s="18">
-        <v>2324</v>
-      </c>
+      <c r="A59" s="18"/>
       <c r="B59" s="21">
         <v>23</v>
       </c>
@@ -6744,9 +6549,7 @@
       <c r="O59" s="3"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A60" s="18">
-        <v>2325</v>
-      </c>
+      <c r="A60" s="18"/>
       <c r="B60" s="21">
         <v>23</v>
       </c>
@@ -6783,9 +6586,7 @@
       <c r="O60" s="3"/>
     </row>
     <row r="61" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="18">
-        <v>2326</v>
-      </c>
+      <c r="A61" s="18"/>
       <c r="B61" s="21">
         <v>23</v>
       </c>
@@ -6822,9 +6623,7 @@
       <c r="O61" s="3"/>
     </row>
     <row r="62" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="18">
-        <v>2327</v>
-      </c>
+      <c r="A62" s="18"/>
       <c r="B62" s="21">
         <v>23</v>
       </c>
@@ -6861,9 +6660,7 @@
       <c r="O62" s="3"/>
     </row>
     <row r="63" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="18">
-        <v>2328</v>
-      </c>
+      <c r="A63" s="18"/>
       <c r="B63" s="21">
         <v>23</v>
       </c>
@@ -6900,9 +6697,7 @@
       <c r="O63" s="3"/>
     </row>
     <row r="64" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A64" s="18">
-        <v>2329</v>
-      </c>
+      <c r="A64" s="18"/>
       <c r="B64" s="21">
         <v>23</v>
       </c>
@@ -6941,9 +6736,7 @@
       <c r="O64" s="3"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A65" s="18">
-        <v>2330</v>
-      </c>
+      <c r="A65" s="18"/>
       <c r="B65" s="21">
         <v>23</v>
       </c>
@@ -6980,9 +6773,7 @@
       <c r="O65" s="3"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A66" s="18">
-        <v>2331</v>
-      </c>
+      <c r="A66" s="18"/>
       <c r="B66" s="21">
         <v>23</v>
       </c>
@@ -7019,9 +6810,7 @@
       <c r="O66" s="3"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A67" s="18">
-        <v>2332</v>
-      </c>
+      <c r="A67" s="18"/>
       <c r="B67" s="21">
         <v>23</v>
       </c>
@@ -7058,9 +6847,7 @@
       <c r="O67" s="3"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A68" s="18">
-        <v>2333</v>
-      </c>
+      <c r="A68" s="18"/>
       <c r="B68" s="21">
         <v>23</v>
       </c>
@@ -7097,9 +6884,7 @@
       <c r="O68" s="3"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A69" s="18">
-        <v>2334</v>
-      </c>
+      <c r="A69" s="18"/>
       <c r="B69" s="21">
         <v>23</v>
       </c>
@@ -7138,9 +6923,7 @@
       <c r="O69" s="3"/>
     </row>
     <row r="70" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="18">
-        <v>2335</v>
-      </c>
+      <c r="A70" s="18"/>
       <c r="B70" s="21">
         <v>23</v>
       </c>
@@ -7177,9 +6960,7 @@
       <c r="O70" s="3"/>
     </row>
     <row r="71" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="18">
-        <v>2336</v>
-      </c>
+      <c r="A71" s="18"/>
       <c r="B71" s="21">
         <v>23</v>
       </c>
@@ -7216,9 +6997,7 @@
       <c r="O71" s="3"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A72" s="18">
-        <v>2337</v>
-      </c>
+      <c r="A72" s="18"/>
       <c r="B72" s="21">
         <v>23</v>
       </c>
@@ -7255,9 +7034,7 @@
       <c r="O72" s="3"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A73" s="18">
-        <v>2338</v>
-      </c>
+      <c r="A73" s="18"/>
       <c r="B73" s="21">
         <v>23</v>
       </c>
@@ -7296,9 +7073,7 @@
       <c r="O73" s="3"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A74" s="18">
-        <v>2339</v>
-      </c>
+      <c r="A74" s="18"/>
       <c r="B74" s="21">
         <v>23</v>
       </c>
@@ -7337,9 +7112,7 @@
       <c r="O74" s="3"/>
     </row>
     <row r="75" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="18">
-        <v>2340</v>
-      </c>
+      <c r="A75" s="18"/>
       <c r="B75" s="21">
         <v>23</v>
       </c>
@@ -7376,9 +7149,7 @@
       <c r="O75" s="3"/>
     </row>
     <row r="76" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A76" s="18">
-        <v>2341</v>
-      </c>
+      <c r="A76" s="18"/>
       <c r="B76" s="21">
         <v>23</v>
       </c>
@@ -7415,9 +7186,7 @@
       <c r="O76" s="3"/>
     </row>
     <row r="77" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A77" s="18">
-        <v>2342</v>
-      </c>
+      <c r="A77" s="18"/>
       <c r="B77" s="21">
         <v>23</v>
       </c>
@@ -7454,9 +7223,7 @@
       <c r="O77" s="3"/>
     </row>
     <row r="78" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A78" s="18">
-        <v>2343</v>
-      </c>
+      <c r="A78" s="18"/>
       <c r="B78" s="21">
         <v>23</v>
       </c>
@@ -7493,9 +7260,7 @@
       <c r="O78" s="3"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A79" s="18">
-        <v>2344</v>
-      </c>
+      <c r="A79" s="18"/>
       <c r="B79" s="21">
         <v>23</v>
       </c>
@@ -7532,9 +7297,7 @@
       <c r="O79" s="3"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A80" s="18">
-        <v>2345</v>
-      </c>
+      <c r="A80" s="18"/>
       <c r="B80" s="21">
         <v>23</v>
       </c>
@@ -7571,9 +7334,7 @@
       <c r="O80" s="3"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A81" s="18">
-        <v>2346</v>
-      </c>
+      <c r="A81" s="18"/>
       <c r="B81" s="21">
         <v>23</v>
       </c>
@@ -7610,9 +7371,7 @@
       <c r="O81" s="3"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A82" s="18">
-        <v>2347</v>
-      </c>
+      <c r="A82" s="18"/>
       <c r="B82" s="21">
         <v>23</v>
       </c>
@@ -7651,9 +7410,7 @@
       <c r="O82" s="3"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A83" s="18">
-        <v>2348</v>
-      </c>
+      <c r="A83" s="18"/>
       <c r="B83" s="21">
         <v>23</v>
       </c>
@@ -7692,9 +7449,7 @@
       <c r="O83" s="3"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A84" s="18">
-        <v>2349</v>
-      </c>
+      <c r="A84" s="18"/>
       <c r="B84" s="21">
         <v>23</v>
       </c>
@@ -7731,9 +7486,7 @@
       <c r="O84" s="3"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A85" s="18">
-        <v>2350</v>
-      </c>
+      <c r="A85" s="18"/>
       <c r="B85" s="21">
         <v>23</v>
       </c>
@@ -7770,9 +7523,7 @@
       <c r="O85" s="3"/>
     </row>
     <row r="86" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A86" s="18">
-        <v>2351</v>
-      </c>
+      <c r="A86" s="18"/>
       <c r="B86" s="21">
         <v>23</v>
       </c>
@@ -7811,9 +7562,7 @@
       <c r="O86" s="3"/>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A87" s="18">
-        <v>2352</v>
-      </c>
+      <c r="A87" s="18"/>
       <c r="B87" s="21">
         <v>23</v>
       </c>
@@ -7850,9 +7599,7 @@
       <c r="O87" s="3"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A88" s="18">
-        <v>2353</v>
-      </c>
+      <c r="A88" s="18"/>
       <c r="B88" s="21">
         <v>23</v>
       </c>
@@ -7889,9 +7636,7 @@
       <c r="O88" s="3"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A89" s="18">
-        <v>2354</v>
-      </c>
+      <c r="A89" s="18"/>
       <c r="B89" s="21">
         <v>23</v>
       </c>
@@ -7930,9 +7675,7 @@
       <c r="O89" s="3"/>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A90" s="18">
-        <v>2355</v>
-      </c>
+      <c r="A90" s="18"/>
       <c r="B90" s="21">
         <v>23</v>
       </c>
@@ -7969,9 +7712,7 @@
       <c r="O90" s="3"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A91" s="18">
-        <v>2356</v>
-      </c>
+      <c r="A91" s="18"/>
       <c r="B91" s="21">
         <v>23</v>
       </c>
@@ -8010,9 +7751,7 @@
       <c r="O91" s="3"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A92" s="18">
-        <v>2357</v>
-      </c>
+      <c r="A92" s="18"/>
       <c r="B92" s="21">
         <v>23</v>
       </c>
@@ -8049,9 +7788,7 @@
       <c r="O92" s="3"/>
     </row>
     <row r="93" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A93" s="18">
-        <v>2358</v>
-      </c>
+      <c r="A93" s="18"/>
       <c r="B93" s="21">
         <v>23</v>
       </c>
@@ -8088,9 +7825,7 @@
       <c r="O93" s="3"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A94" s="18">
-        <v>2401</v>
-      </c>
+      <c r="A94" s="18"/>
       <c r="B94" s="20">
         <v>24</v>
       </c>
@@ -8127,9 +7862,7 @@
       <c r="O94" s="3"/>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A95" s="18">
-        <v>2402</v>
-      </c>
+      <c r="A95" s="18"/>
       <c r="B95" s="20">
         <v>24</v>
       </c>
@@ -8166,9 +7899,7 @@
       <c r="O95" s="3"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A96" s="18">
-        <v>2403</v>
-      </c>
+      <c r="A96" s="18"/>
       <c r="B96" s="20">
         <v>24</v>
       </c>
@@ -8205,9 +7936,7 @@
       <c r="O96" s="3"/>
     </row>
     <row r="97" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A97" s="18">
-        <v>2404</v>
-      </c>
+      <c r="A97" s="18"/>
       <c r="B97" s="20">
         <v>24</v>
       </c>
@@ -8244,9 +7973,7 @@
       <c r="O97" s="3"/>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A98" s="18">
-        <v>2405</v>
-      </c>
+      <c r="A98" s="18"/>
       <c r="B98" s="20">
         <v>24</v>
       </c>
@@ -8283,9 +8010,7 @@
       <c r="O98" s="3"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A99" s="18">
-        <v>2406</v>
-      </c>
+      <c r="A99" s="18"/>
       <c r="B99" s="20">
         <v>24</v>
       </c>
@@ -8322,9 +8047,7 @@
       <c r="O99" s="3"/>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A100" s="18">
-        <v>2407</v>
-      </c>
+      <c r="A100" s="18"/>
       <c r="B100" s="20">
         <v>24</v>
       </c>
@@ -8361,9 +8084,7 @@
       <c r="O100" s="3"/>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A101" s="18">
-        <v>2408</v>
-      </c>
+      <c r="A101" s="18"/>
       <c r="B101" s="20">
         <v>24</v>
       </c>
@@ -8400,9 +8121,7 @@
       <c r="O101" s="3"/>
     </row>
     <row r="102" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A102" s="18">
-        <v>2409</v>
-      </c>
+      <c r="A102" s="18"/>
       <c r="B102" s="20">
         <v>24</v>
       </c>
@@ -8439,9 +8158,7 @@
       <c r="O102" s="3"/>
     </row>
     <row r="103" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A103" s="18">
-        <v>2410</v>
-      </c>
+      <c r="A103" s="18"/>
       <c r="B103" s="20">
         <v>24</v>
       </c>
@@ -8478,9 +8195,7 @@
       <c r="O103" s="3"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A104" s="18">
-        <v>2411</v>
-      </c>
+      <c r="A104" s="18"/>
       <c r="B104" s="20">
         <v>24</v>
       </c>
@@ -8517,9 +8232,7 @@
       <c r="O104" s="3"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A105" s="18">
-        <v>2501</v>
-      </c>
+      <c r="A105" s="18"/>
       <c r="B105" s="19">
         <v>25</v>
       </c>
@@ -8556,9 +8269,7 @@
       <c r="O105" s="3"/>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A106" s="18">
-        <v>2502</v>
-      </c>
+      <c r="A106" s="18"/>
       <c r="B106" s="19">
         <v>25</v>
       </c>
@@ -8595,9 +8306,7 @@
       <c r="O106" s="3"/>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A107" s="18">
-        <v>2503</v>
-      </c>
+      <c r="A107" s="18"/>
       <c r="B107" s="19">
         <v>25</v>
       </c>
@@ -8634,9 +8343,7 @@
       <c r="O107" s="3"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A108" s="18">
-        <v>2504</v>
-      </c>
+      <c r="A108" s="18"/>
       <c r="B108" s="19">
         <v>25</v>
       </c>
@@ -8673,9 +8380,7 @@
       <c r="O108" s="3"/>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A109" s="18">
-        <v>4101</v>
-      </c>
+      <c r="A109" s="18"/>
       <c r="B109" s="18">
         <v>41</v>
       </c>
@@ -8712,9 +8417,7 @@
       <c r="O109" s="3"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A110" s="18">
-        <v>9901</v>
-      </c>
+      <c r="A110" s="18"/>
       <c r="B110" s="4" t="s">
         <v>301</v>
       </c>
@@ -8753,9 +8456,7 @@
       <c r="O110" s="3"/>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A111" s="18">
-        <v>9902</v>
-      </c>
+      <c r="A111" s="18"/>
       <c r="B111" s="4" t="s">
         <v>301</v>
       </c>
@@ -8794,9 +8495,7 @@
       <c r="O111" s="3"/>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A112" s="18">
-        <v>9903</v>
-      </c>
+      <c r="A112" s="18"/>
       <c r="B112" s="4" t="s">
         <v>301</v>
       </c>
@@ -8835,9 +8534,7 @@
       <c r="O112" s="3"/>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A113" s="18">
-        <v>9904</v>
-      </c>
+      <c r="A113" s="18"/>
       <c r="B113" s="4" t="s">
         <v>301</v>
       </c>
@@ -8876,9 +8573,7 @@
       <c r="O113" s="3"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A114" s="18">
-        <v>9905</v>
-      </c>
+      <c r="A114" s="18"/>
       <c r="B114" s="4" t="s">
         <v>301</v>
       </c>
@@ -8917,9 +8612,7 @@
       <c r="O114" s="3"/>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A115" s="18">
-        <v>9906</v>
-      </c>
+      <c r="A115" s="18"/>
       <c r="B115" s="4" t="s">
         <v>301</v>
       </c>
@@ -8958,9 +8651,7 @@
       <c r="O115" s="3"/>
     </row>
     <row r="116" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A116" s="18">
-        <v>9911</v>
-      </c>
+      <c r="A116" s="18"/>
       <c r="B116" s="4" t="s">
         <v>301</v>
       </c>
@@ -9001,9 +8692,7 @@
       <c r="O116" s="3"/>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A117" s="18">
-        <v>9912</v>
-      </c>
+      <c r="A117" s="18"/>
       <c r="B117" s="4" t="s">
         <v>301</v>
       </c>
@@ -9042,9 +8731,7 @@
       <c r="O117" s="3"/>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A118" s="18">
-        <v>9913</v>
-      </c>
+      <c r="A118" s="18"/>
       <c r="B118" s="4" t="s">
         <v>301</v>
       </c>
@@ -9083,9 +8770,7 @@
       <c r="O118" s="3"/>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A119" s="18">
-        <v>9914</v>
-      </c>
+      <c r="A119" s="18"/>
       <c r="B119" s="4" t="s">
         <v>301</v>
       </c>
@@ -9124,9 +8809,7 @@
       <c r="O119" s="3"/>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A120" s="18">
-        <v>9915</v>
-      </c>
+      <c r="A120" s="18"/>
       <c r="B120" s="4" t="s">
         <v>301</v>
       </c>
@@ -9165,9 +8848,7 @@
       <c r="O120" s="3"/>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A121" s="18">
-        <v>9916</v>
-      </c>
+      <c r="A121" s="18"/>
       <c r="B121" s="4" t="s">
         <v>301</v>
       </c>
@@ -9206,9 +8887,7 @@
       <c r="O121" s="3"/>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A122" s="18">
-        <v>9921</v>
-      </c>
+      <c r="A122" s="18"/>
       <c r="B122" s="4" t="s">
         <v>301</v>
       </c>
@@ -9247,9 +8926,7 @@
       <c r="O122" s="3"/>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A123" s="18">
-        <v>9922</v>
-      </c>
+      <c r="A123" s="18"/>
       <c r="B123" s="4" t="s">
         <v>301</v>
       </c>
@@ -9288,9 +8965,7 @@
       <c r="O123" s="3"/>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A124" s="18">
-        <v>9923</v>
-      </c>
+      <c r="A124" s="18"/>
       <c r="B124" s="4" t="s">
         <v>301</v>
       </c>
@@ -9329,9 +9004,7 @@
       <c r="O124" s="3"/>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A125" s="18">
-        <v>9924</v>
-      </c>
+      <c r="A125" s="18"/>
       <c r="B125" s="4" t="s">
         <v>301</v>
       </c>
@@ -9370,9 +9043,7 @@
       <c r="O125" s="3"/>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A126" s="18">
-        <v>9925</v>
-      </c>
+      <c r="A126" s="18"/>
       <c r="B126" s="4" t="s">
         <v>301</v>
       </c>
@@ -9411,9 +9082,7 @@
       <c r="O126" s="3"/>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A127" s="18">
-        <v>9926</v>
-      </c>
+      <c r="A127" s="18"/>
       <c r="B127" s="4" t="s">
         <v>301</v>
       </c>
@@ -9452,9 +9121,7 @@
       <c r="O127" s="3"/>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A128" s="18">
-        <v>9931</v>
-      </c>
+      <c r="A128" s="18"/>
       <c r="B128" s="4" t="s">
         <v>301</v>
       </c>
@@ -9493,9 +9160,7 @@
       <c r="O128" s="3"/>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A129" s="18">
-        <v>9932</v>
-      </c>
+      <c r="A129" s="18"/>
       <c r="B129" s="4" t="s">
         <v>301</v>
       </c>
@@ -9534,9 +9199,7 @@
       <c r="O129" s="3"/>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A130" s="18">
-        <v>9933</v>
-      </c>
+      <c r="A130" s="18"/>
       <c r="B130" s="4" t="s">
         <v>301</v>
       </c>
@@ -9575,9 +9238,7 @@
       <c r="O130" s="3"/>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A131" s="18">
-        <v>9934</v>
-      </c>
+      <c r="A131" s="18"/>
       <c r="B131" s="4" t="s">
         <v>301</v>
       </c>
@@ -9616,9 +9277,7 @@
       <c r="O131" s="3"/>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A132" s="18">
-        <v>9935</v>
-      </c>
+      <c r="A132" s="18"/>
       <c r="B132" s="4" t="s">
         <v>301</v>
       </c>
@@ -9657,9 +9316,7 @@
       <c r="O132" s="3"/>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A133" s="18">
-        <v>9936</v>
-      </c>
+      <c r="A133" s="18"/>
       <c r="B133" s="4" t="s">
         <v>301</v>
       </c>
@@ -9698,9 +9355,7 @@
       <c r="O133" s="3"/>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A134" s="18">
-        <v>9941</v>
-      </c>
+      <c r="A134" s="18"/>
       <c r="B134" s="4" t="s">
         <v>301</v>
       </c>
@@ -9739,9 +9394,7 @@
       <c r="O134" s="3"/>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A135" s="18">
-        <v>9942</v>
-      </c>
+      <c r="A135" s="18"/>
       <c r="B135" s="4" t="s">
         <v>301</v>
       </c>
@@ -9780,9 +9433,7 @@
       <c r="O135" s="3"/>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A136" s="18">
-        <v>9943</v>
-      </c>
+      <c r="A136" s="18"/>
       <c r="B136" s="4" t="s">
         <v>301</v>
       </c>
@@ -9821,9 +9472,7 @@
       <c r="O136" s="3"/>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A137" s="18">
-        <v>9944</v>
-      </c>
+      <c r="A137" s="18"/>
       <c r="B137" s="4" t="s">
         <v>301</v>
       </c>
@@ -9862,9 +9511,7 @@
       <c r="O137" s="3"/>
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A138" s="18">
-        <v>9945</v>
-      </c>
+      <c r="A138" s="18"/>
       <c r="B138" s="4" t="s">
         <v>301</v>
       </c>
@@ -9903,9 +9550,7 @@
       <c r="O138" s="3"/>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A139" s="18">
-        <v>9946</v>
-      </c>
+      <c r="A139" s="18"/>
       <c r="B139" s="4" t="s">
         <v>301</v>
       </c>
@@ -9956,7 +9601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA261AD-49AF-4AB4-9B1D-D659E636DAE8}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -9967,91 +9612,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
+        <v>472</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>460</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>462</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>464</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>466</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>468</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" s="29" t="s">
         <v>473</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="27">
-        <v>1</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>461</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="27">
-        <v>2</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>463</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="27">
-        <v>3</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>465</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="27">
-        <v>4</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>467</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="27">
-        <v>5</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>469</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="27">
-        <v>6</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>471</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
-        <v>7</v>
-      </c>
-      <c r="B8" s="30" t="s">
+      <c r="C8" s="30" t="s">
         <v>474</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>